<commit_message>
added maximum run duration and calculation for mass of foam
</commit_message>
<xml_diff>
--- a/ENGR290_BOM.xlsx
+++ b/ENGR290_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\Documents\GitHub\ENGR290_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B42492-47C2-42F9-AB1A-1EE39A26E70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44874692-CCE0-411F-AA39-3412C95F1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA2E9C97-5D3C-4CB7-ABB0-53836FD0B0E6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>part number</t>
   </si>
@@ -44,9 +44,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>dimensions</t>
-  </si>
-  <si>
     <t>voltage needed (V)</t>
   </si>
   <si>
@@ -96,6 +93,24 @@
   </si>
   <si>
     <t>total power consumption in mW</t>
+  </si>
+  <si>
+    <t>Power budget of batteries</t>
+  </si>
+  <si>
+    <t>7.2V * 180mAh * 2 = 2592mWh</t>
+  </si>
+  <si>
+    <t>weight of the foam in kg</t>
+  </si>
+  <si>
+    <t>volume of the foam in cm^3</t>
+  </si>
+  <si>
+    <t>maximum run duration in hrs</t>
+  </si>
+  <si>
+    <t>maximum run duration in minutes</t>
   </si>
 </sst>
 </file>
@@ -447,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CBFEE6-8CAC-4479-8FBE-8FDAB83CC443}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,11 +474,14 @@
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,27 +489,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -506,13 +527,21 @@
         <f>D2*E2</f>
         <v>38.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <f>PI() * 2.5 * (45/2)^2</f>
+        <v>3976.0782021995819</v>
+      </c>
+      <c r="I2">
+        <f>(H2/1000000)*30</f>
+        <v>0.11928234606598745</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -528,12 +557,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -549,12 +578,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -570,12 +599,12 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -591,12 +620,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -612,15 +641,35 @@
         <v>12.54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
         <f>SUM(F2:F7)</f>
         <v>5770.94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <f>(2592/A10)</f>
+        <v>0.44914693273539497</v>
+      </c>
+      <c r="G10">
+        <f>F10*60</f>
+        <v>26.948815964123696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expanded spreadsheet to have some mass and dimensions
</commit_message>
<xml_diff>
--- a/ENGR290_BOM.xlsx
+++ b/ENGR290_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\Documents\GitHub\ENGR290_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44874692-CCE0-411F-AA39-3412C95F1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E407E-DDCB-4CBC-8373-71E9BBCA78D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA2E9C97-5D3C-4CB7-ABB0-53836FD0B0E6}"/>
+    <workbookView xWindow="-96" yWindow="3456" windowWidth="17280" windowHeight="8880" xr2:uid="{AA2E9C97-5D3C-4CB7-ABB0-53836FD0B0E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>part number</t>
   </si>
@@ -111,6 +111,30 @@
   </si>
   <si>
     <t>maximum run duration in minutes</t>
+  </si>
+  <si>
+    <t>batteries</t>
+  </si>
+  <si>
+    <t>turnigy nano-tech 180mAh 2s</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>mass (g)</t>
+  </si>
+  <si>
+    <t>dimensions (cm lxwxh)</t>
+  </si>
+  <si>
+    <t>3.5x2.0x1.0</t>
+  </si>
+  <si>
+    <t>foam</t>
+  </si>
+  <si>
+    <t>45x45x2.5</t>
   </si>
 </sst>
 </file>
@@ -462,15 +486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CBFEE6-8CAC-4479-8FBE-8FDAB83CC443}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
@@ -481,7 +505,7 @@
     <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,14 +524,20 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -527,16 +557,16 @@
         <f>D2*E2</f>
         <v>38.4</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <f>PI() * 2.5 * (45/2)^2</f>
         <v>3976.0782021995819</v>
       </c>
-      <c r="I2">
-        <f>(H2/1000000)*30</f>
+      <c r="K2">
+        <f>(J2/1000000)*30</f>
         <v>0.11928234606598745</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -557,7 +587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -578,7 +608,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -599,7 +629,7 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -620,7 +650,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -641,34 +671,86 @@
         <v>12.54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>119</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
         <f>SUM(F2:F7)</f>
         <v>5770.94</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="F10">
-        <f>(2592/A10)</f>
+      <c r="F12">
+        <f>(2592/A12)</f>
         <v>0.44914693273539497</v>
       </c>
-      <c r="G10">
-        <f>F10*60</f>
+      <c r="G12">
+        <f>F12*60</f>
         <v>26.948815964123696</v>
       </c>
     </row>

</xml_diff>